<commit_message>
feat: using new template
</commit_message>
<xml_diff>
--- a/asserts/coords_tracking/PETALBURG CITY coordinates.xlsx
+++ b/asserts/coords_tracking/PETALBURG CITY coordinates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SS\Documents\GitHub\pokemmo_py_auto\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SS\Documents\GitHub\pokemmo_py_auto\asserts\coords_tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF5F5B1-9DA7-4B25-B1F5-3880478ADAC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C008415-30D2-491A-B615-7EFECD2C5D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,14 @@
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="1">
+  <si>
+    <t>farming</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,15 +388,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL21"/>
+  <dimension ref="A1:AU21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AU9" sqref="AU9"/>
+      <selection activeCell="AW8" sqref="AW8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>7</v>
       </c>
@@ -500,8 +508,35 @@
       <c r="AL1" s="1">
         <v>43</v>
       </c>
+      <c r="AM1" s="1">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>45</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>47</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>48</v>
+      </c>
+      <c r="AR1" s="1">
+        <v>49</v>
+      </c>
+      <c r="AS1" s="1">
+        <v>50</v>
+      </c>
+      <c r="AT1" s="1">
+        <v>51</v>
+      </c>
+      <c r="AU1" s="1">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>9</v>
       </c>
@@ -557,7 +592,7 @@
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
     </row>
-    <row r="3" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -611,7 +646,7 @@
       <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
     </row>
-    <row r="4" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>11</v>
       </c>
@@ -667,7 +702,7 @@
       <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
     </row>
-    <row r="5" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>12</v>
       </c>
@@ -706,14 +741,14 @@
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
-      <c r="AG5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="2">
-        <v>1</v>
+      <c r="AG5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AJ5" s="2">
         <v>1</v>
@@ -724,8 +759,32 @@
       <c r="AL5" s="2">
         <v>1</v>
       </c>
+      <c r="AM5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AR5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AS5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU5" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>13</v>
       </c>
@@ -782,14 +841,14 @@
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
-      <c r="AG6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="2">
-        <v>1</v>
+      <c r="AG6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AJ6" s="2">
         <v>1</v>
@@ -800,8 +859,35 @@
       <c r="AL6" s="2">
         <v>1</v>
       </c>
+      <c r="AM6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AP6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AR6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AS6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU6" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>14</v>
       </c>
@@ -856,32 +942,32 @@
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
-      <c r="AA7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI7" s="2">
-        <v>1</v>
+      <c r="AA7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AJ7" s="2">
         <v>1</v>
@@ -892,8 +978,32 @@
       <c r="AL7" s="2">
         <v>1</v>
       </c>
+      <c r="AM7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AP7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AS7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU7" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>15</v>
       </c>
@@ -942,29 +1052,29 @@
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
-      <c r="AA8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH8" s="2">
-        <v>1</v>
+      <c r="AA8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AI8" s="2">
         <v>1</v>
@@ -978,8 +1088,35 @@
       <c r="AL8" s="2">
         <v>1</v>
       </c>
+      <c r="AM8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AP8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AR8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AS8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU8" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>16</v>
       </c>
@@ -1039,26 +1176,26 @@
       <c r="AA9" s="2">
         <v>1</v>
       </c>
-      <c r="AB9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH9" s="2">
-        <v>1</v>
+      <c r="AB9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AI9" s="2">
         <v>1</v>
@@ -1073,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>17</v>
       </c>
@@ -1144,17 +1281,17 @@
       <c r="AB10" s="2">
         <v>1</v>
       </c>
-      <c r="AC10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="2">
-        <v>1</v>
+      <c r="AC10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2">
@@ -1173,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>18</v>
       </c>
@@ -1271,7 +1408,7 @@
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
     </row>
-    <row r="12" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>19</v>
       </c>
@@ -1353,7 +1490,7 @@
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
     </row>
-    <row r="13" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -1429,7 +1566,7 @@
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
     </row>
-    <row r="14" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>21</v>
       </c>
@@ -1483,7 +1620,7 @@
       <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
     </row>
-    <row r="15" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>22</v>
       </c>
@@ -1530,11 +1667,11 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
-      <c r="AE15" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF15" s="2">
-        <v>1</v>
+      <c r="AE15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AG15" s="2">
         <v>1</v>
@@ -1547,7 +1684,7 @@
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
     </row>
-    <row r="16" spans="1:38" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>23</v>
       </c>
@@ -1590,11 +1727,11 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
-      <c r="AE16" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF16" s="2">
-        <v>1</v>
+      <c r="AE16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
@@ -1644,14 +1781,14 @@
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
-      <c r="AE17" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF17" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG17" s="2">
-        <v>1</v>
+      <c r="AE17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AH17" s="2">
         <v>1</v>
@@ -1720,14 +1857,14 @@
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
-      <c r="AE18" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF18" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG18" s="2">
-        <v>1</v>
+      <c r="AE18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AH18" s="2">
         <v>1</v>
@@ -1794,17 +1931,17 @@
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
-      <c r="AE19" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF19" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG19" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH19" s="2">
-        <v>1</v>
+      <c r="AE19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
@@ -1866,17 +2003,17 @@
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
-      <c r="AE20" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF20" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG20" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH20" s="2">
-        <v>1</v>
+      <c r="AE20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>

</xml_diff>